<commit_message>
algoritmos para compilação dos mapas
</commit_message>
<xml_diff>
--- a/output/semivariogram-models-sif.xlsx
+++ b/output/semivariogram-models-sif.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,55 +419,22 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.0237</v>
+        <v>0.0303</v>
       </c>
       <c r="E2">
-        <v>0.9564</v>
+        <v>0.1458</v>
       </c>
       <c r="F2">
-        <v>1931.01</v>
+        <v>219.96</v>
       </c>
       <c r="G2">
-        <v>0.02478042659974905</v>
+        <v>0.2078189300411522</v>
       </c>
       <c r="H2">
-        <v>0.0004</v>
+        <v>0.0183</v>
       </c>
       <c r="I2">
-        <v>0.3496</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PA</t>
-        </is>
-      </c>
-      <c r="B3">
-        <v>2015</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Sph</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>0.0149</v>
-      </c>
-      <c r="E3">
-        <v>0.0226</v>
-      </c>
-      <c r="F3">
-        <v>3.33</v>
-      </c>
-      <c r="G3">
-        <v>0.6592920353982301</v>
-      </c>
-      <c r="H3">
-        <v>0.0005999999999999999</v>
-      </c>
-      <c r="I3">
-        <v>0.1289</v>
+        <v>-1.112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xco2 e sif parcial
</commit_message>
<xml_diff>
--- a/output/semivariogram-models-sif.xlsx
+++ b/output/semivariogram-models-sif.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="B2">
@@ -419,22 +419,913 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.0303</v>
+        <v>0.0168</v>
       </c>
       <c r="E2">
-        <v>0.1458</v>
+        <v>0.3721</v>
       </c>
       <c r="F2">
-        <v>219.96</v>
+        <v>172.68</v>
       </c>
       <c r="G2">
-        <v>0.2078189300411522</v>
+        <v>0.04514915345337274</v>
       </c>
       <c r="H2">
-        <v>0.0183</v>
+        <v>0.0045</v>
       </c>
       <c r="I2">
-        <v>-1.112</v>
+        <v>0.1826</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2016</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.021</v>
+      </c>
+      <c r="E3">
+        <v>0.5053</v>
+      </c>
+      <c r="F3">
+        <v>302.14</v>
+      </c>
+      <c r="G3">
+        <v>0.04155946962200673</v>
+      </c>
+      <c r="H3">
+        <v>0.0052</v>
+      </c>
+      <c r="I3">
+        <v>0.0583</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.037</v>
+      </c>
+      <c r="E4">
+        <v>0.0579</v>
+      </c>
+      <c r="F4">
+        <v>2.75</v>
+      </c>
+      <c r="G4">
+        <v>0.6390328151986183</v>
+      </c>
+      <c r="H4">
+        <v>0.0062</v>
+      </c>
+      <c r="I4">
+        <v>-0.0496</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2018</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.0175</v>
+      </c>
+      <c r="E5">
+        <v>0.3502</v>
+      </c>
+      <c r="F5">
+        <v>193.1</v>
+      </c>
+      <c r="G5">
+        <v>0.04997144488863507</v>
+      </c>
+      <c r="H5">
+        <v>0.0034</v>
+      </c>
+      <c r="I5">
+        <v>-0.5404</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2019</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.0469</v>
+      </c>
+      <c r="E6">
+        <v>0.8743</v>
+      </c>
+      <c r="F6">
+        <v>87.75</v>
+      </c>
+      <c r="G6">
+        <v>0.05364291433146517</v>
+      </c>
+      <c r="H6">
+        <v>0.0587</v>
+      </c>
+      <c r="I6">
+        <v>-0.0397</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.135</v>
+      </c>
+      <c r="E7">
+        <v>6978.5458</v>
+      </c>
+      <c r="F7">
+        <v>2084.89</v>
+      </c>
+      <c r="G7">
+        <v>1.934500451369109E-05</v>
+      </c>
+      <c r="H7">
+        <v>0.0822</v>
+      </c>
+      <c r="I7">
+        <v>-8.2607</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>2015</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.0499</v>
+      </c>
+      <c r="E8">
+        <v>643.3389</v>
+      </c>
+      <c r="F8">
+        <v>1178.08</v>
+      </c>
+      <c r="G8">
+        <v>7.756409568891296E-05</v>
+      </c>
+      <c r="H8">
+        <v>0.0252</v>
+      </c>
+      <c r="I8">
+        <v>-1.5117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>2016</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.0366</v>
+      </c>
+      <c r="E9">
+        <v>0.0992</v>
+      </c>
+      <c r="F9">
+        <v>140.02</v>
+      </c>
+      <c r="G9">
+        <v>0.3689516129032258</v>
+      </c>
+      <c r="H9">
+        <v>0.0189</v>
+      </c>
+      <c r="I9">
+        <v>-7.4572</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2017</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.0644</v>
+      </c>
+      <c r="F10">
+        <v>1.56</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.0062</v>
+      </c>
+      <c r="I10">
+        <v>-0.2493</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.0202</v>
+      </c>
+      <c r="E11">
+        <v>0.5212</v>
+      </c>
+      <c r="F11">
+        <v>342.47</v>
+      </c>
+      <c r="G11">
+        <v>0.03875671527244819</v>
+      </c>
+      <c r="H11">
+        <v>0.0043</v>
+      </c>
+      <c r="I11">
+        <v>-0.1762</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>2019</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.0221</v>
+      </c>
+      <c r="E12">
+        <v>0.0604</v>
+      </c>
+      <c r="F12">
+        <v>7.08</v>
+      </c>
+      <c r="G12">
+        <v>0.3658940397350994</v>
+      </c>
+      <c r="H12">
+        <v>0.0028</v>
+      </c>
+      <c r="I12">
+        <v>0.2536</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MG</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>2020</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.0081</v>
+      </c>
+      <c r="E13">
+        <v>0.0835</v>
+      </c>
+      <c r="F13">
+        <v>2.15</v>
+      </c>
+      <c r="G13">
+        <v>0.09700598802395208</v>
+      </c>
+      <c r="H13">
+        <v>2.5401</v>
+      </c>
+      <c r="I13">
+        <v>-4.4597</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>2015</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.04</v>
+      </c>
+      <c r="F14">
+        <v>0.28</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.0007</v>
+      </c>
+      <c r="I14">
+        <v>-0.2789</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>2016</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>0.0145</v>
+      </c>
+      <c r="E15">
+        <v>0.1777</v>
+      </c>
+      <c r="F15">
+        <v>125.85</v>
+      </c>
+      <c r="G15">
+        <v>0.08159819921215532</v>
+      </c>
+      <c r="H15">
+        <v>0.0003</v>
+      </c>
+      <c r="I15">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>2017</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>0.0668</v>
+      </c>
+      <c r="E16">
+        <v>0.1188</v>
+      </c>
+      <c r="F16">
+        <v>20.46</v>
+      </c>
+      <c r="G16">
+        <v>0.5622895622895623</v>
+      </c>
+      <c r="H16">
+        <v>0.06619999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.2479</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>2018</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>0.0143</v>
+      </c>
+      <c r="E17">
+        <v>0.0338</v>
+      </c>
+      <c r="F17">
+        <v>16.11</v>
+      </c>
+      <c r="G17">
+        <v>0.4230769230769231</v>
+      </c>
+      <c r="H17">
+        <v>0.0004</v>
+      </c>
+      <c r="I17">
+        <v>-0.0806</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>2019</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>0.0196</v>
+      </c>
+      <c r="E18">
+        <v>0.06419999999999999</v>
+      </c>
+      <c r="F18">
+        <v>5.08</v>
+      </c>
+      <c r="G18">
+        <v>0.3052959501557633</v>
+      </c>
+      <c r="H18">
+        <v>0.0014</v>
+      </c>
+      <c r="I18">
+        <v>0.4453</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>2020</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>0.07049999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.6444</v>
+      </c>
+      <c r="F19">
+        <v>32.2</v>
+      </c>
+      <c r="G19">
+        <v>0.1094040968342644</v>
+      </c>
+      <c r="H19">
+        <v>55.1642</v>
+      </c>
+      <c r="I19">
+        <v>-1.2066</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>2015</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D20">
+        <v>0.0246</v>
+      </c>
+      <c r="E20">
+        <v>0.0392</v>
+      </c>
+      <c r="F20">
+        <v>12.67</v>
+      </c>
+      <c r="G20">
+        <v>0.6275510204081632</v>
+      </c>
+      <c r="H20">
+        <v>0.0003</v>
+      </c>
+      <c r="I20">
+        <v>0.2819</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>2016</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D21">
+        <v>0.0142</v>
+      </c>
+      <c r="E21">
+        <v>0.0291</v>
+      </c>
+      <c r="F21">
+        <v>1.72</v>
+      </c>
+      <c r="G21">
+        <v>0.4879725085910653</v>
+      </c>
+      <c r="H21">
+        <v>0.0016</v>
+      </c>
+      <c r="I21">
+        <v>0.07240000000000001</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>2017</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D22">
+        <v>0.0206</v>
+      </c>
+      <c r="E22">
+        <v>0.0534</v>
+      </c>
+      <c r="F22">
+        <v>11.03</v>
+      </c>
+      <c r="G22">
+        <v>0.3857677902621723</v>
+      </c>
+      <c r="H22">
+        <v>0.0021</v>
+      </c>
+      <c r="I22">
+        <v>-0.0291</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>2018</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D23">
+        <v>0.0396</v>
+      </c>
+      <c r="E23">
+        <v>0.0487</v>
+      </c>
+      <c r="F23">
+        <v>51.08</v>
+      </c>
+      <c r="G23">
+        <v>0.8131416837782341</v>
+      </c>
+      <c r="H23">
+        <v>0.0046</v>
+      </c>
+      <c r="I23">
+        <v>-0.1256</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>2019</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D24">
+        <v>0.0365</v>
+      </c>
+      <c r="E24">
+        <v>0.1721</v>
+      </c>
+      <c r="F24">
+        <v>71.8</v>
+      </c>
+      <c r="G24">
+        <v>0.2120859965136548</v>
+      </c>
+      <c r="H24">
+        <v>0.0077</v>
+      </c>
+      <c r="I24">
+        <v>0.2441</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>2020</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0.2544</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.1494</v>
+      </c>
+      <c r="I25">
+        <v>-0.0411</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B26">
+        <v>2015</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D26">
+        <v>0.0158</v>
+      </c>
+      <c r="E26">
+        <v>0.0257</v>
+      </c>
+      <c r="F26">
+        <v>9.6</v>
+      </c>
+      <c r="G26">
+        <v>0.6147859922178989</v>
+      </c>
+      <c r="H26">
+        <v>0.0013</v>
+      </c>
+      <c r="I26">
+        <v>0.0168</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B27">
+        <v>2016</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D27">
+        <v>0.011</v>
+      </c>
+      <c r="E27">
+        <v>0.0259</v>
+      </c>
+      <c r="F27">
+        <v>2.01</v>
+      </c>
+      <c r="G27">
+        <v>0.4247104247104247</v>
+      </c>
+      <c r="H27">
+        <v>0.0008</v>
+      </c>
+      <c r="I27">
+        <v>0.1136</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B28">
+        <v>2017</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D28">
+        <v>0.0353</v>
+      </c>
+      <c r="E28">
+        <v>0.0486</v>
+      </c>
+      <c r="F28">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0.7263374485596708</v>
+      </c>
+      <c r="H28">
+        <v>0.0018</v>
+      </c>
+      <c r="I28">
+        <v>0.6766</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B29">
+        <v>2018</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="D29">
+        <v>0.0259</v>
+      </c>
+      <c r="E29">
+        <v>0.0404</v>
+      </c>
+      <c r="F29">
+        <v>4.92</v>
+      </c>
+      <c r="G29">
+        <v>0.6410891089108911</v>
+      </c>
+      <c r="H29">
+        <v>0.0023</v>
+      </c>
+      <c r="I29">
+        <v>0.283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novos mapas e correção do cálculo dos Betas
</commit_message>
<xml_diff>
--- a/output/semivariogram-models-sif.xlsx
+++ b/output/semivariogram-models-sif.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,26 +415,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Gau</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.0168</v>
+        <v>0.0322</v>
       </c>
       <c r="E2">
-        <v>0.3721</v>
+        <v>1038.8228</v>
       </c>
       <c r="F2">
-        <v>172.68</v>
+        <v>1236.24</v>
       </c>
       <c r="G2">
-        <v>0.04514915345337274</v>
+        <v>3.099662425584037E-05</v>
       </c>
       <c r="H2">
-        <v>0.0045</v>
+        <v>0.0232</v>
       </c>
       <c r="I2">
-        <v>0.1826</v>
+        <v>-1.2087</v>
       </c>
     </row>
     <row r="3">
@@ -452,22 +452,22 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.021</v>
+        <v>0.0194</v>
       </c>
       <c r="E3">
-        <v>0.5053</v>
+        <v>0.4549</v>
       </c>
       <c r="F3">
-        <v>302.14</v>
+        <v>240.19</v>
       </c>
       <c r="G3">
-        <v>0.04155946962200673</v>
+        <v>0.0426467355462739</v>
       </c>
       <c r="H3">
-        <v>0.0052</v>
+        <v>0.0061</v>
       </c>
       <c r="I3">
-        <v>0.0583</v>
+        <v>0.2022</v>
       </c>
     </row>
     <row r="4">
@@ -485,22 +485,22 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.037</v>
+        <v>0.0385</v>
       </c>
       <c r="E4">
-        <v>0.0579</v>
+        <v>0.0575</v>
       </c>
       <c r="F4">
-        <v>2.75</v>
+        <v>2.66</v>
       </c>
       <c r="G4">
-        <v>0.6390328151986183</v>
+        <v>0.6695652173913043</v>
       </c>
       <c r="H4">
-        <v>0.0062</v>
+        <v>0.0067</v>
       </c>
       <c r="I4">
-        <v>-0.0496</v>
+        <v>-0.2834</v>
       </c>
     </row>
     <row r="5">
@@ -518,22 +518,22 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.0175</v>
+        <v>0.0187</v>
       </c>
       <c r="E5">
-        <v>0.3502</v>
+        <v>0.4214</v>
       </c>
       <c r="F5">
-        <v>193.1</v>
+        <v>277.87</v>
       </c>
       <c r="G5">
-        <v>0.04997144488863507</v>
+        <v>0.04437588989084006</v>
       </c>
       <c r="H5">
-        <v>0.0034</v>
+        <v>0.0033</v>
       </c>
       <c r="I5">
-        <v>-0.5404</v>
+        <v>-0.3111</v>
       </c>
     </row>
     <row r="6">
@@ -547,26 +547,26 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Gau</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.0469</v>
+        <v>0.0684</v>
       </c>
       <c r="E6">
-        <v>0.8743</v>
+        <v>0.1702</v>
       </c>
       <c r="F6">
-        <v>87.75</v>
+        <v>8.49</v>
       </c>
       <c r="G6">
-        <v>0.05364291433146517</v>
+        <v>0.4018801410105758</v>
       </c>
       <c r="H6">
-        <v>0.0587</v>
+        <v>0.048</v>
       </c>
       <c r="I6">
-        <v>-0.0397</v>
+        <v>-0.4541</v>
       </c>
     </row>
     <row r="7">
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.135</v>
+        <v>0.1362</v>
       </c>
       <c r="E7">
-        <v>6978.5458</v>
+        <v>2190.6024</v>
       </c>
       <c r="F7">
-        <v>2084.89</v>
+        <v>1152.64</v>
       </c>
       <c r="G7">
-        <v>1.934500451369109E-05</v>
+        <v>6.217467852678331E-05</v>
       </c>
       <c r="H7">
-        <v>0.0822</v>
+        <v>0.0849</v>
       </c>
       <c r="I7">
-        <v>-8.2607</v>
+        <v>-11.57</v>
       </c>
     </row>
     <row r="8">
@@ -613,26 +613,26 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Gau</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D8">
-        <v>0.0499</v>
+        <v>0.0269</v>
       </c>
       <c r="E8">
-        <v>643.3389</v>
+        <v>0.575</v>
       </c>
       <c r="F8">
-        <v>1178.08</v>
+        <v>321.68</v>
       </c>
       <c r="G8">
-        <v>7.756409568891296E-05</v>
+        <v>0.04678260869565218</v>
       </c>
       <c r="H8">
-        <v>0.0252</v>
+        <v>0.0323</v>
       </c>
       <c r="I8">
-        <v>-1.5117</v>
+        <v>-0.1488</v>
       </c>
     </row>
     <row r="9">
@@ -650,22 +650,22 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.0366</v>
+        <v>0.0247</v>
       </c>
       <c r="E9">
-        <v>0.0992</v>
+        <v>0.2812</v>
       </c>
       <c r="F9">
-        <v>140.02</v>
+        <v>286.22</v>
       </c>
       <c r="G9">
-        <v>0.3689516129032258</v>
+        <v>0.08783783783783783</v>
       </c>
       <c r="H9">
-        <v>0.0189</v>
+        <v>0.0037</v>
       </c>
       <c r="I9">
-        <v>-7.4572</v>
+        <v>-1.1299</v>
       </c>
     </row>
     <row r="10">
@@ -679,17 +679,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0.0644</v>
+        <v>0.06279999999999999</v>
       </c>
       <c r="F10">
-        <v>1.56</v>
+        <v>1.51</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>0.0062</v>
       </c>
       <c r="I10">
-        <v>-0.2493</v>
+        <v>-0.3295</v>
       </c>
     </row>
     <row r="11">
@@ -716,22 +716,22 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.0202</v>
+        <v>0.0181</v>
       </c>
       <c r="E11">
-        <v>0.5212</v>
+        <v>0.3724</v>
       </c>
       <c r="F11">
-        <v>342.47</v>
+        <v>193.37</v>
       </c>
       <c r="G11">
-        <v>0.03875671527244819</v>
+        <v>0.04860365198711063</v>
       </c>
       <c r="H11">
-        <v>0.0043</v>
+        <v>0.0049</v>
       </c>
       <c r="I11">
-        <v>-0.1762</v>
+        <v>-0.1237</v>
       </c>
     </row>
     <row r="12">
@@ -749,22 +749,22 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.0221</v>
+        <v>0.0225</v>
       </c>
       <c r="E12">
-        <v>0.0604</v>
+        <v>0.0751</v>
       </c>
       <c r="F12">
-        <v>7.08</v>
+        <v>8.94</v>
       </c>
       <c r="G12">
-        <v>0.3658940397350994</v>
+        <v>0.2996005326231691</v>
       </c>
       <c r="H12">
-        <v>0.0028</v>
+        <v>0.0025</v>
       </c>
       <c r="I12">
-        <v>0.2536</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="13">
@@ -778,26 +778,26 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Gau</t>
         </is>
       </c>
       <c r="D13">
-        <v>0.0081</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.0835</v>
+        <v>0.3547</v>
       </c>
       <c r="F13">
-        <v>2.15</v>
+        <v>1.26</v>
       </c>
       <c r="G13">
-        <v>0.09700598802395208</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>2.5401</v>
+        <v>0.2104</v>
       </c>
       <c r="I13">
-        <v>-4.4597</v>
+        <v>-0.0008</v>
       </c>
     </row>
     <row r="14">
@@ -811,26 +811,26 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Gau</t>
         </is>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.0391</v>
       </c>
       <c r="E14">
-        <v>0.04</v>
+        <v>0.0408</v>
       </c>
       <c r="F14">
-        <v>0.28</v>
+        <v>0.87</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="H14">
-        <v>0.0007</v>
+        <v>0.0003</v>
       </c>
       <c r="I14">
-        <v>-0.2789</v>
+        <v>-0.2209</v>
       </c>
     </row>
     <row r="15">
@@ -844,26 +844,26 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D15">
-        <v>0.0145</v>
+        <v>0.0151</v>
       </c>
       <c r="E15">
-        <v>0.1777</v>
+        <v>0.8643</v>
       </c>
       <c r="F15">
-        <v>125.85</v>
+        <v>1240.14</v>
       </c>
       <c r="G15">
-        <v>0.08159819921215532</v>
+        <v>0.01747078560684947</v>
       </c>
       <c r="H15">
-        <v>0.0003</v>
+        <v>0.0004</v>
       </c>
       <c r="I15">
-        <v>0.214</v>
+        <v>0.0711</v>
       </c>
     </row>
     <row r="16">
@@ -881,22 +881,22 @@
         </is>
       </c>
       <c r="D16">
-        <v>0.0668</v>
+        <v>0.0285</v>
       </c>
       <c r="E16">
-        <v>0.1188</v>
+        <v>0.1778</v>
       </c>
       <c r="F16">
-        <v>20.46</v>
+        <v>25.07</v>
       </c>
       <c r="G16">
-        <v>0.5622895622895623</v>
+        <v>0.1602924634420697</v>
       </c>
       <c r="H16">
-        <v>0.06619999999999999</v>
+        <v>0.0224</v>
       </c>
       <c r="I16">
-        <v>0.2479</v>
+        <v>0.2542</v>
       </c>
     </row>
     <row r="17">
@@ -910,26 +910,26 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Gau</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D17">
-        <v>0.0143</v>
+        <v>0.0142</v>
       </c>
       <c r="E17">
-        <v>0.0338</v>
+        <v>0.4584</v>
       </c>
       <c r="F17">
-        <v>16.11</v>
+        <v>551.42</v>
       </c>
       <c r="G17">
-        <v>0.4230769230769231</v>
+        <v>0.03097731239092496</v>
       </c>
       <c r="H17">
-        <v>0.0004</v>
+        <v>0.0019</v>
       </c>
       <c r="I17">
-        <v>-0.0806</v>
+        <v>-3.2505</v>
       </c>
     </row>
     <row r="18">
@@ -943,26 +943,26 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D18">
-        <v>0.0196</v>
+        <v>0.0126</v>
       </c>
       <c r="E18">
-        <v>0.06419999999999999</v>
+        <v>0.075</v>
       </c>
       <c r="F18">
-        <v>5.08</v>
+        <v>8.130000000000001</v>
       </c>
       <c r="G18">
-        <v>0.3052959501557633</v>
+        <v>0.168</v>
       </c>
       <c r="H18">
-        <v>0.0014</v>
+        <v>0.0017</v>
       </c>
       <c r="I18">
-        <v>0.4453</v>
+        <v>0.4811</v>
       </c>
     </row>
     <row r="19">
@@ -980,22 +980,22 @@
         </is>
       </c>
       <c r="D19">
-        <v>0.07049999999999999</v>
+        <v>0.0132</v>
       </c>
       <c r="E19">
-        <v>0.6444</v>
+        <v>0.0674</v>
       </c>
       <c r="F19">
-        <v>32.2</v>
+        <v>15.19</v>
       </c>
       <c r="G19">
-        <v>0.1094040968342644</v>
+        <v>0.1958456973293768</v>
       </c>
       <c r="H19">
-        <v>55.1642</v>
+        <v>65.9798</v>
       </c>
       <c r="I19">
-        <v>-1.2066</v>
+        <v>-5.4748</v>
       </c>
     </row>
     <row r="20">
@@ -1009,26 +1009,26 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Gau</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D20">
-        <v>0.0246</v>
+        <v>0.0219</v>
       </c>
       <c r="E20">
-        <v>0.0392</v>
+        <v>0.4571</v>
       </c>
       <c r="F20">
-        <v>12.67</v>
+        <v>447.34</v>
       </c>
       <c r="G20">
-        <v>0.6275510204081632</v>
+        <v>0.047910741632028</v>
       </c>
       <c r="H20">
-        <v>0.0003</v>
+        <v>0.0048</v>
       </c>
       <c r="I20">
-        <v>0.2819</v>
+        <v>-0.7625999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1046,22 +1046,22 @@
         </is>
       </c>
       <c r="D21">
-        <v>0.0142</v>
+        <v>0.0171</v>
       </c>
       <c r="E21">
-        <v>0.0291</v>
+        <v>0.029</v>
       </c>
       <c r="F21">
-        <v>1.72</v>
+        <v>2.34</v>
       </c>
       <c r="G21">
-        <v>0.4879725085910653</v>
+        <v>0.5896551724137931</v>
       </c>
       <c r="H21">
-        <v>0.0016</v>
+        <v>0.002</v>
       </c>
       <c r="I21">
-        <v>0.07240000000000001</v>
+        <v>-0.1081</v>
       </c>
     </row>
     <row r="22">
@@ -1075,26 +1075,26 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D22">
-        <v>0.0206</v>
+        <v>0.0209</v>
       </c>
       <c r="E22">
-        <v>0.0534</v>
+        <v>3.9107</v>
       </c>
       <c r="F22">
-        <v>11.03</v>
+        <v>2730.17</v>
       </c>
       <c r="G22">
-        <v>0.3857677902621723</v>
+        <v>0.00534431176004295</v>
       </c>
       <c r="H22">
         <v>0.0021</v>
       </c>
       <c r="I22">
-        <v>-0.0291</v>
+        <v>0.2872</v>
       </c>
     </row>
     <row r="23">
@@ -1108,26 +1108,26 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D23">
-        <v>0.0396</v>
+        <v>0.0332</v>
       </c>
       <c r="E23">
-        <v>0.0487</v>
+        <v>0.2548</v>
       </c>
       <c r="F23">
-        <v>51.08</v>
+        <v>350.21</v>
       </c>
       <c r="G23">
-        <v>0.8131416837782341</v>
+        <v>0.130298273155416</v>
       </c>
       <c r="H23">
-        <v>0.0046</v>
+        <v>0.0067</v>
       </c>
       <c r="I23">
-        <v>-0.1256</v>
+        <v>-2.0969</v>
       </c>
     </row>
     <row r="24">
@@ -1141,26 +1141,26 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sph</t>
+          <t>Gau</t>
         </is>
       </c>
       <c r="D24">
-        <v>0.0365</v>
+        <v>0.0393</v>
       </c>
       <c r="E24">
-        <v>0.1721</v>
+        <v>218.8241</v>
       </c>
       <c r="F24">
-        <v>71.8</v>
+        <v>1124.81</v>
       </c>
       <c r="G24">
-        <v>0.2120859965136548</v>
+        <v>0.0001795963058913529</v>
       </c>
       <c r="H24">
-        <v>0.0077</v>
+        <v>0.0066</v>
       </c>
       <c r="I24">
-        <v>0.2441</v>
+        <v>-0.0325</v>
       </c>
     </row>
     <row r="25">
@@ -1178,22 +1178,22 @@
         </is>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.2031</v>
       </c>
       <c r="E25">
-        <v>0.2544</v>
+        <v>698.9262</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>583.16</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>0.0002905886200860692</v>
       </c>
       <c r="H25">
-        <v>0.1494</v>
+        <v>0.08160000000000001</v>
       </c>
       <c r="I25">
-        <v>-0.0411</v>
+        <v>0.5056</v>
       </c>
     </row>
     <row r="26">
@@ -1207,26 +1207,26 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="D26">
-        <v>0.0158</v>
+        <v>0.0181</v>
       </c>
       <c r="E26">
-        <v>0.0257</v>
+        <v>0.0314</v>
       </c>
       <c r="F26">
-        <v>9.6</v>
+        <v>19.18</v>
       </c>
       <c r="G26">
-        <v>0.6147859922178989</v>
+        <v>0.5764331210191084</v>
       </c>
       <c r="H26">
-        <v>0.0013</v>
+        <v>0.0002</v>
       </c>
       <c r="I26">
-        <v>0.0168</v>
+        <v>0.7635</v>
       </c>
     </row>
     <row r="27">
@@ -1240,26 +1240,26 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="D27">
-        <v>0.011</v>
+        <v>0.0224</v>
       </c>
       <c r="E27">
-        <v>0.0259</v>
+        <v>0.0266</v>
       </c>
       <c r="F27">
-        <v>2.01</v>
+        <v>6.2</v>
       </c>
       <c r="G27">
-        <v>0.4247104247104247</v>
+        <v>0.8421052631578948</v>
       </c>
       <c r="H27">
-        <v>0.0008</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="I27">
-        <v>0.1136</v>
+        <v>0.1653</v>
       </c>
     </row>
     <row r="28">
@@ -1273,26 +1273,26 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Gau</t>
+          <t>Exp</t>
         </is>
       </c>
       <c r="D28">
-        <v>0.0353</v>
+        <v>0.0338</v>
       </c>
       <c r="E28">
-        <v>0.0486</v>
+        <v>0.126</v>
       </c>
       <c r="F28">
-        <v>9.380000000000001</v>
+        <v>153.54</v>
       </c>
       <c r="G28">
-        <v>0.7263374485596708</v>
+        <v>0.2682539682539682</v>
       </c>
       <c r="H28">
-        <v>0.0018</v>
+        <v>0.0009</v>
       </c>
       <c r="I28">
-        <v>0.6766</v>
+        <v>0.7718</v>
       </c>
     </row>
     <row r="29">
@@ -1306,26 +1306,92 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>Sph</t>
         </is>
       </c>
       <c r="D29">
-        <v>0.0259</v>
+        <v>0.0302</v>
       </c>
       <c r="E29">
-        <v>0.0404</v>
+        <v>0.0398</v>
       </c>
       <c r="F29">
-        <v>4.92</v>
+        <v>4.79</v>
       </c>
       <c r="G29">
-        <v>0.6410891089108911</v>
+        <v>0.7587939698492462</v>
       </c>
       <c r="H29">
-        <v>0.0023</v>
+        <v>0.0015</v>
       </c>
       <c r="I29">
-        <v>0.283</v>
+        <v>0.3411</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B30">
+        <v>2019</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D30">
+        <v>0.0159</v>
+      </c>
+      <c r="E30">
+        <v>0.0505</v>
+      </c>
+      <c r="F30">
+        <v>1.26</v>
+      </c>
+      <c r="G30">
+        <v>0.3148514851485149</v>
+      </c>
+      <c r="H30">
+        <v>0.0097</v>
+      </c>
+      <c r="I30">
+        <v>-0.146</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B31">
+        <v>2020</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Gau</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0.2465</v>
+      </c>
+      <c r="F31">
+        <v>3.22</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0.0687</v>
+      </c>
+      <c r="I31">
+        <v>0.0675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>